<commit_message>
More clustering and interval options
More clustering and interval options
</commit_message>
<xml_diff>
--- a/inputData/Blue_wOrange_V1.xlsx
+++ b/inputData/Blue_wOrange_V1.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unmm-my.sharepoint.com/personal/majic_unm_edu/Documents/Disertacion Marzo 2020/Second Empirical Paper 2022/Analysis 2023/inputData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{852504DD-5CAA-421E-8833-2E79F45CAB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{440BB84F-1D12-4270-88A6-ADB25D55E46A}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{852504DD-5CAA-421E-8833-2E79F45CAB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B91AC90D-7DEF-4A85-9A8F-80D636F4FF12}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blue_Video_1_2023" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blue_Video_1_2023!$1:$198</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blue_Video_1_2023!$1:$197</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="36">
   <si>
     <t>Sync Time</t>
   </si>
@@ -136,11 +136,23 @@
   <si>
     <t>Index</t>
   </si>
+  <si>
+    <t>Red_1_14</t>
+  </si>
+  <si>
+    <t>Red_1_15</t>
+  </si>
+  <si>
+    <t>Red_1_16</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm:ss.000"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -283,7 +295,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -463,8 +475,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -579,6 +597,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -624,9 +670,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -683,6 +733,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -982,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XEX198"/>
+  <dimension ref="A1:XEX233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="J191" sqref="J191"/>
+    <sheetView tabSelected="1" topLeftCell="A184" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A221" sqref="A221:E233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1472,16 +1526,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>3.8923611111111116E-3</v>
+        <v>3.9363425925925928E-3</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29">
         <v>3</v>
@@ -1489,16 +1543,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>3.9305555555555561E-3</v>
+        <v>3.9467592592592592E-3</v>
       </c>
       <c r="B30" t="s">
         <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30">
         <v>3</v>
@@ -1506,16 +1560,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>3.9467592592592592E-3</v>
+        <v>4.108796296296297E-3</v>
       </c>
       <c r="B31" t="s">
         <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E31">
         <v>3</v>
@@ -1523,16 +1577,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>4.108796296296297E-3</v>
+        <v>4.153935185185185E-3</v>
       </c>
       <c r="B32" t="s">
         <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D32">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -1540,16 +1594,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>4.153935185185185E-3</v>
+        <v>4.1967592592592586E-3</v>
       </c>
       <c r="B33" t="s">
         <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E33">
         <v>3</v>
@@ -1557,16 +1611,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>4.1967592592592586E-3</v>
+        <v>4.2060185185185187E-3</v>
       </c>
       <c r="B34" t="s">
         <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D34">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E34">
         <v>3</v>
@@ -1574,7 +1628,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>4.2060185185185187E-3</v>
+        <v>4.6307870370370366E-3</v>
       </c>
       <c r="B35" t="s">
         <v>13</v>
@@ -1591,33 +1645,33 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>4.5868055555555558E-3</v>
+        <v>6.2743055555555564E-3</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E36">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>6.2743055555555564E-3</v>
+        <v>6.2766203703703708E-3</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D37">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E37">
         <v>4</v>
@@ -1625,16 +1679,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>6.2766203703703708E-3</v>
+        <v>6.2881944444444443E-3</v>
       </c>
       <c r="B38" t="s">
         <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E38">
         <v>4</v>
@@ -1642,16 +1696,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>6.2881944444444443E-3</v>
+        <v>6.2986111111111116E-3</v>
       </c>
       <c r="B39" t="s">
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D39">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E39">
         <v>4</v>
@@ -1659,16 +1713,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
-        <v>6.2986111111111116E-3</v>
+        <v>6.3101851851851852E-3</v>
       </c>
       <c r="B40" t="s">
         <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E40">
         <v>4</v>
@@ -1676,16 +1730,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>6.3101851851851852E-3</v>
+        <v>6.3159722222222228E-3</v>
       </c>
       <c r="B41" t="s">
         <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D41">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E41">
         <v>4</v>
@@ -1693,16 +1747,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
-        <v>6.3159722222222228E-3</v>
+        <v>6.3298611111111116E-3</v>
       </c>
       <c r="B42" t="s">
         <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E42">
         <v>4</v>
@@ -1710,16 +1764,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
-        <v>6.3298611111111116E-3</v>
+        <v>6.3460648148148148E-3</v>
       </c>
       <c r="B43" t="s">
         <v>15</v>
       </c>
       <c r="C43" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D43">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E43">
         <v>4</v>
@@ -1727,16 +1781,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
-        <v>6.3460648148148148E-3</v>
+        <v>6.363425925925926E-3</v>
       </c>
       <c r="B44" t="s">
         <v>15</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E44">
         <v>4</v>
@@ -1744,16 +1798,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
-        <v>6.363425925925926E-3</v>
+        <v>6.3877314814814812E-3</v>
       </c>
       <c r="B45" t="s">
         <v>15</v>
       </c>
       <c r="C45" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D45">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E45">
         <v>4</v>
@@ -1761,16 +1815,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
-        <v>6.3877314814814812E-3</v>
+        <v>6.4745370370370382E-3</v>
       </c>
       <c r="B46" t="s">
         <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E46">
         <v>4</v>
@@ -1778,16 +1832,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
-        <v>6.4745370370370382E-3</v>
+        <v>6.5254629629629629E-3</v>
       </c>
       <c r="B47" t="s">
         <v>15</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D47">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E47">
         <v>4</v>
@@ -1795,16 +1849,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
-        <v>6.5254629629629629E-3</v>
+        <v>6.533564814814815E-3</v>
       </c>
       <c r="B48" t="s">
         <v>15</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E48">
         <v>4</v>
@@ -1812,16 +1866,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
-        <v>6.533564814814815E-3</v>
+        <v>6.5659722222222222E-3</v>
       </c>
       <c r="B49" t="s">
         <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E49">
         <v>4</v>
@@ -1829,16 +1883,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
-        <v>6.5659722222222222E-3</v>
+        <v>6.5752314814814814E-3</v>
       </c>
       <c r="B50" t="s">
         <v>15</v>
       </c>
       <c r="C50" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E50">
         <v>4</v>
@@ -1846,16 +1900,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
-        <v>6.5752314814814814E-3</v>
+        <v>6.5833333333333334E-3</v>
       </c>
       <c r="B51" t="s">
         <v>15</v>
       </c>
       <c r="C51" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D51">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E51">
         <v>4</v>
@@ -1863,16 +1917,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
-        <v>6.5833333333333334E-3</v>
+        <v>6.594907407407407E-3</v>
       </c>
       <c r="B52" t="s">
         <v>15</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E52">
         <v>4</v>
@@ -1880,16 +1934,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
-        <v>6.594907407407407E-3</v>
+        <v>6.6215277777777783E-3</v>
       </c>
       <c r="B53" t="s">
         <v>15</v>
       </c>
       <c r="C53" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D53">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E53">
         <v>4</v>
@@ -1897,16 +1951,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
-        <v>6.6215277777777783E-3</v>
+        <v>6.6504629629629622E-3</v>
       </c>
       <c r="B54" t="s">
         <v>15</v>
       </c>
       <c r="C54" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E54">
         <v>4</v>
@@ -1914,16 +1968,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
-        <v>6.6504629629629622E-3</v>
+        <v>6.6782407407407415E-3</v>
       </c>
       <c r="B55" t="s">
         <v>15</v>
       </c>
       <c r="C55" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D55">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E55">
         <v>4</v>
@@ -1931,16 +1985,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
-        <v>6.6782407407407415E-3</v>
+        <v>6.7268518518518519E-3</v>
       </c>
       <c r="B56" t="s">
         <v>15</v>
       </c>
       <c r="C56" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E56">
         <v>4</v>
@@ -1948,16 +2002,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
-        <v>6.7268518518518519E-3</v>
+        <v>6.7488425925925936E-3</v>
       </c>
       <c r="B57" t="s">
         <v>15</v>
       </c>
       <c r="C57" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E57">
         <v>4</v>
@@ -1965,16 +2019,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
-        <v>6.7488425925925936E-3</v>
+        <v>6.8680555555555552E-3</v>
       </c>
       <c r="B58" t="s">
         <v>15</v>
       </c>
       <c r="C58" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E58">
         <v>4</v>
@@ -1982,16 +2036,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
-        <v>6.8680555555555552E-3</v>
+        <v>6.9120370370370368E-3</v>
       </c>
       <c r="B59" t="s">
         <v>15</v>
       </c>
       <c r="C59" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E59">
         <v>4</v>
@@ -1999,16 +2053,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
-        <v>6.9120370370370368E-3</v>
+        <v>6.9351851851851857E-3</v>
       </c>
       <c r="B60" t="s">
         <v>15</v>
       </c>
       <c r="C60" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E60">
         <v>4</v>
@@ -2016,7 +2070,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
-        <v>6.9351851851851857E-3</v>
+        <v>6.9687500000000001E-3</v>
       </c>
       <c r="B61" t="s">
         <v>15</v>
@@ -2033,33 +2087,33 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
-        <v>6.9687500000000001E-3</v>
+        <v>7.8599537037037041E-3</v>
       </c>
       <c r="B62" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C62" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D62">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E62">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
-        <v>7.8599537037037041E-3</v>
+        <v>7.8935185185185185E-3</v>
       </c>
       <c r="B63" t="s">
         <v>22</v>
       </c>
       <c r="C63" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E63">
         <v>5</v>
@@ -2067,16 +2121,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
-        <v>7.8935185185185185E-3</v>
+        <v>7.9166666666666673E-3</v>
       </c>
       <c r="B64" t="s">
         <v>22</v>
       </c>
       <c r="C64" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D64">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E64">
         <v>5</v>
@@ -2084,16 +2138,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
-        <v>7.9166666666666673E-3</v>
+        <v>7.9317129629629633E-3</v>
       </c>
       <c r="B65" t="s">
         <v>22</v>
       </c>
       <c r="C65" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E65">
         <v>5</v>
@@ -2101,16 +2155,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
-        <v>7.9317129629629633E-3</v>
+        <v>8.0138888888888881E-3</v>
       </c>
       <c r="B66" t="s">
         <v>22</v>
       </c>
       <c r="C66" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D66">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E66">
         <v>5</v>
@@ -2118,16 +2172,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
-        <v>8.0138888888888881E-3</v>
+        <v>8.3622685185185171E-3</v>
       </c>
       <c r="B67" t="s">
         <v>22</v>
       </c>
       <c r="C67" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="E67">
         <v>5</v>
@@ -2135,16 +2189,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
-        <v>8.3622685185185171E-3</v>
+        <v>8.3993055555555557E-3</v>
       </c>
       <c r="B68" t="s">
         <v>22</v>
       </c>
       <c r="C68" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D68">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="E68">
         <v>5</v>
@@ -2152,16 +2206,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
-        <v>8.3993055555555557E-3</v>
+        <v>8.416666666666666E-3</v>
       </c>
       <c r="B69" t="s">
         <v>22</v>
       </c>
       <c r="C69" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D69">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E69">
         <v>5</v>
@@ -2169,16 +2223,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
-        <v>8.416666666666666E-3</v>
+        <v>8.4259259259259253E-3</v>
       </c>
       <c r="B70" t="s">
         <v>22</v>
       </c>
       <c r="C70" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E70">
         <v>5</v>
@@ -2186,16 +2240,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
-        <v>8.4259259259259253E-3</v>
+        <v>8.487268518518519E-3</v>
       </c>
       <c r="B71" t="s">
         <v>22</v>
       </c>
       <c r="C71" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D71">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E71">
         <v>5</v>
@@ -2203,16 +2257,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
-        <v>8.487268518518519E-3</v>
+        <v>8.5416666666666679E-3</v>
       </c>
       <c r="B72" t="s">
         <v>22</v>
       </c>
       <c r="C72" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D72">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E72">
         <v>5</v>
@@ -2220,16 +2274,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
-        <v>8.5416666666666679E-3</v>
+        <v>8.5474537037037047E-3</v>
       </c>
       <c r="B73" t="s">
         <v>22</v>
       </c>
       <c r="C73" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D73">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E73">
         <v>5</v>
@@ -2237,7 +2291,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
-        <v>8.5474537037037047E-3</v>
+        <v>8.5543981481481478E-3</v>
       </c>
       <c r="B74" t="s">
         <v>22</v>
@@ -2254,33 +2308,33 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
-        <v>8.5543981481481478E-3</v>
+        <v>9.0532407407407419E-3</v>
       </c>
       <c r="B75" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C75" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D75">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E75">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
-        <v>9.0532407407407419E-3</v>
+        <v>9.0682870370370362E-3</v>
       </c>
       <c r="B76" t="s">
         <v>23</v>
       </c>
       <c r="C76" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D76">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E76">
         <v>6</v>
@@ -2288,16 +2342,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
-        <v>9.0682870370370362E-3</v>
+        <v>9.0798611111111097E-3</v>
       </c>
       <c r="B77" t="s">
         <v>23</v>
       </c>
       <c r="C77" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D77">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E77">
         <v>6</v>
@@ -2305,16 +2359,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
-        <v>9.0798611111111097E-3</v>
+        <v>9.2048611111111116E-3</v>
       </c>
       <c r="B78" t="s">
         <v>23</v>
       </c>
       <c r="C78" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D78">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E78">
         <v>6</v>
@@ -2322,16 +2376,16 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
-        <v>9.2048611111111116E-3</v>
+        <v>9.2303240740740731E-3</v>
       </c>
       <c r="B79" t="s">
         <v>23</v>
       </c>
       <c r="C79" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E79">
         <v>6</v>
@@ -2339,16 +2393,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
-        <v>9.2303240740740731E-3</v>
+        <v>9.2824074074074076E-3</v>
       </c>
       <c r="B80" t="s">
         <v>23</v>
       </c>
       <c r="C80" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D80">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E80">
         <v>6</v>
@@ -2356,16 +2410,16 @@
     </row>
     <row r="81" spans="1:5 16378:16378" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
-        <v>9.2824074074074076E-3</v>
+        <v>9.3032407407407404E-3</v>
       </c>
       <c r="B81" t="s">
         <v>23</v>
       </c>
       <c r="C81" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E81">
         <v>6</v>
@@ -2373,16 +2427,16 @@
     </row>
     <row r="82" spans="1:5 16378:16378" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
-        <v>9.3032407407407404E-3</v>
+        <v>9.3090277777777772E-3</v>
       </c>
       <c r="B82" t="s">
         <v>23</v>
       </c>
       <c r="C82" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D82">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E82">
         <v>6</v>
@@ -2390,16 +2444,16 @@
     </row>
     <row r="83" spans="1:5 16378:16378" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
-        <v>9.3090277777777772E-3</v>
+        <v>9.3287037037037036E-3</v>
       </c>
       <c r="B83" t="s">
         <v>23</v>
       </c>
       <c r="C83" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D83">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E83">
         <v>6</v>
@@ -2407,16 +2461,16 @@
     </row>
     <row r="84" spans="1:5 16378:16378" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
-        <v>9.3287037037037036E-3</v>
+        <v>9.3344907407407404E-3</v>
       </c>
       <c r="B84" t="s">
         <v>23</v>
       </c>
       <c r="C84" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D84">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E84">
         <v>6</v>
@@ -2424,16 +2478,16 @@
     </row>
     <row r="85" spans="1:5 16378:16378" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
-        <v>9.3344907407407404E-3</v>
+        <v>9.618055555555555E-3</v>
       </c>
       <c r="B85" t="s">
         <v>23</v>
       </c>
       <c r="C85" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D85">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E85">
         <v>6</v>
@@ -2441,16 +2495,16 @@
     </row>
     <row r="86" spans="1:5 16378:16378" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
-        <v>9.618055555555555E-3</v>
+        <v>9.6273148148148142E-3</v>
       </c>
       <c r="B86" t="s">
         <v>23</v>
       </c>
       <c r="C86" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D86">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E86">
         <v>6</v>
@@ -2458,16 +2512,16 @@
     </row>
     <row r="87" spans="1:5 16378:16378" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
-        <v>9.6273148148148142E-3</v>
+        <v>9.6712962962962959E-3</v>
       </c>
       <c r="B87" t="s">
         <v>23</v>
       </c>
       <c r="C87" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D87">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E87">
         <v>6</v>
@@ -2475,16 +2529,16 @@
     </row>
     <row r="88" spans="1:5 16378:16378" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
-        <v>9.6712962962962959E-3</v>
+        <v>9.6909722222222223E-3</v>
       </c>
       <c r="B88" t="s">
         <v>23</v>
       </c>
       <c r="C88" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D88">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E88">
         <v>6</v>
@@ -2492,16 +2546,16 @@
     </row>
     <row r="89" spans="1:5 16378:16378" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
-        <v>9.6909722222222223E-3</v>
+        <v>9.7430555555555552E-3</v>
       </c>
       <c r="B89" t="s">
         <v>23</v>
       </c>
       <c r="C89" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D89">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E89">
         <v>6</v>
@@ -2509,7 +2563,7 @@
     </row>
     <row r="90" spans="1:5 16378:16378" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
-        <v>9.7430555555555552E-3</v>
+        <v>9.7476851851851856E-3</v>
       </c>
       <c r="B90" t="s">
         <v>23</v>
@@ -2526,53 +2580,53 @@
     </row>
     <row r="91" spans="1:5 16378:16378" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
-        <v>9.7476851851851856E-3</v>
+        <v>1.1137731481481483E-2</v>
       </c>
       <c r="B91" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C91" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D91">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E91">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="XEX91" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="92" spans="1:5 16378:16378" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
-        <v>1.1137731481481483E-2</v>
+        <v>1.1155092592592591E-2</v>
       </c>
       <c r="B92" t="s">
         <v>25</v>
       </c>
       <c r="C92" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D92">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E92">
         <v>7</v>
-      </c>
-      <c r="XEX92" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="93" spans="1:5 16378:16378" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
-        <v>1.1155092592592591E-2</v>
+        <v>1.1174768518518516E-2</v>
       </c>
       <c r="B93" t="s">
         <v>25</v>
       </c>
       <c r="C93" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D93">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E93">
         <v>7</v>
@@ -2580,16 +2634,16 @@
     </row>
     <row r="94" spans="1:5 16378:16378" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
-        <v>1.1174768518518516E-2</v>
+        <v>1.119097222222222E-2</v>
       </c>
       <c r="B94" t="s">
         <v>25</v>
       </c>
       <c r="C94" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D94">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E94">
         <v>7</v>
@@ -2597,16 +2651,16 @@
     </row>
     <row r="95" spans="1:5 16378:16378" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
-        <v>1.119097222222222E-2</v>
+        <v>1.1230324074074073E-2</v>
       </c>
       <c r="B95" t="s">
         <v>25</v>
       </c>
       <c r="C95" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D95">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E95">
         <v>7</v>
@@ -2614,16 +2668,16 @@
     </row>
     <row r="96" spans="1:5 16378:16378" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
-        <v>1.1230324074074073E-2</v>
+        <v>1.1291666666666667E-2</v>
       </c>
       <c r="B96" t="s">
         <v>25</v>
       </c>
       <c r="C96" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D96">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E96">
         <v>7</v>
@@ -2631,16 +2685,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
-        <v>1.1291666666666667E-2</v>
+        <v>1.1320601851851851E-2</v>
       </c>
       <c r="B97" t="s">
         <v>25</v>
       </c>
       <c r="C97" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D97">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E97">
         <v>7</v>
@@ -2648,16 +2702,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
-        <v>1.1320601851851851E-2</v>
+        <v>1.1326388888888888E-2</v>
       </c>
       <c r="B98" t="s">
         <v>25</v>
       </c>
       <c r="C98" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D98">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E98">
         <v>7</v>
@@ -2665,16 +2719,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
-        <v>1.1326388888888888E-2</v>
+        <v>1.134375E-2</v>
       </c>
       <c r="B99" t="s">
         <v>25</v>
       </c>
       <c r="C99" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D99">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E99">
         <v>7</v>
@@ -2682,16 +2736,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
-        <v>1.134375E-2</v>
+        <v>1.1386574074074075E-2</v>
       </c>
       <c r="B100" t="s">
         <v>25</v>
       </c>
       <c r="C100" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D100">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E100">
         <v>7</v>
@@ -2699,16 +2753,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
-        <v>1.1386574074074075E-2</v>
+        <v>1.1395833333333334E-2</v>
       </c>
       <c r="B101" t="s">
         <v>25</v>
       </c>
       <c r="C101" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D101">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E101">
         <v>7</v>
@@ -2716,16 +2770,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
-        <v>1.1395833333333334E-2</v>
+        <v>1.1459490740740741E-2</v>
       </c>
       <c r="B102" t="s">
         <v>25</v>
       </c>
       <c r="C102" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E102">
         <v>7</v>
@@ -2733,16 +2787,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
-        <v>1.1459490740740741E-2</v>
+        <v>1.1482638888888889E-2</v>
       </c>
       <c r="B103" t="s">
         <v>25</v>
       </c>
       <c r="C103" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D103">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E103">
         <v>7</v>
@@ -2750,16 +2804,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
-        <v>1.1482638888888889E-2</v>
+        <v>1.1511574074074075E-2</v>
       </c>
       <c r="B104" t="s">
         <v>25</v>
       </c>
       <c r="C104" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D104">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E104">
         <v>7</v>
@@ -2767,16 +2821,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
-        <v>1.1511574074074075E-2</v>
+        <v>1.1528935185185185E-2</v>
       </c>
       <c r="B105" t="s">
         <v>25</v>
       </c>
       <c r="C105" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D105">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E105">
         <v>7</v>
@@ -2784,16 +2838,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
-        <v>1.1528935185185185E-2</v>
+        <v>1.1673611111111109E-2</v>
       </c>
       <c r="B106" t="s">
         <v>25</v>
       </c>
       <c r="C106" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E106">
         <v>7</v>
@@ -2801,16 +2855,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
-        <v>1.1673611111111109E-2</v>
+        <v>1.1701388888888891E-2</v>
       </c>
       <c r="B107" t="s">
         <v>25</v>
       </c>
       <c r="C107" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D107">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E107">
         <v>7</v>
@@ -2818,16 +2872,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
-        <v>1.1701388888888891E-2</v>
+        <v>1.1768518518518518E-2</v>
       </c>
       <c r="B108" t="s">
         <v>25</v>
       </c>
       <c r="C108" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D108">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E108">
         <v>7</v>
@@ -2835,7 +2889,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
-        <v>1.1768518518518518E-2</v>
+        <v>1.1832175925925927E-2</v>
       </c>
       <c r="B109" t="s">
         <v>25</v>
@@ -2852,10 +2906,10 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
-        <v>1.1832175925925927E-2</v>
+        <v>1.218287037037037E-2</v>
       </c>
       <c r="B110" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C110" t="s">
         <v>7</v>
@@ -2864,21 +2918,21 @@
         <v>1</v>
       </c>
       <c r="E110">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
-        <v>1.218287037037037E-2</v>
+        <v>1.2453703703703703E-2</v>
       </c>
       <c r="B111" t="s">
         <v>26</v>
       </c>
       <c r="C111" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D111">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E111">
         <v>8</v>
@@ -2886,16 +2940,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
-        <v>1.2453703703703703E-2</v>
+        <v>1.2505787037037037E-2</v>
       </c>
       <c r="B112" t="s">
         <v>26</v>
       </c>
       <c r="C112" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D112">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E112">
         <v>8</v>
@@ -2903,16 +2957,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
-        <v>1.2505787037037037E-2</v>
+        <v>1.2525462962962962E-2</v>
       </c>
       <c r="B113" t="s">
         <v>26</v>
       </c>
       <c r="C113" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D113">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E113">
         <v>8</v>
@@ -2920,16 +2974,16 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
-        <v>1.2525462962962962E-2</v>
+        <v>1.2548611111111113E-2</v>
       </c>
       <c r="B114" t="s">
         <v>26</v>
       </c>
       <c r="C114" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D114">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="E114">
         <v>8</v>
@@ -2937,16 +2991,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
-        <v>1.2548611111111113E-2</v>
+        <v>1.2575231481481481E-2</v>
       </c>
       <c r="B115" t="s">
         <v>26</v>
       </c>
       <c r="C115" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D115">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E115">
         <v>8</v>
@@ -2954,16 +3008,16 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
-        <v>1.2575231481481481E-2</v>
+        <v>1.2728009259259258E-2</v>
       </c>
       <c r="B116" t="s">
         <v>26</v>
       </c>
       <c r="C116" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D116">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E116">
         <v>8</v>
@@ -2971,16 +3025,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
-        <v>1.2728009259259258E-2</v>
+        <v>1.2841435185185185E-2</v>
       </c>
       <c r="B117" t="s">
         <v>26</v>
       </c>
       <c r="C117" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D117">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E117">
         <v>8</v>
@@ -2988,16 +3042,16 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
-        <v>1.2841435185185185E-2</v>
+        <v>1.2855324074074075E-2</v>
       </c>
       <c r="B118" t="s">
         <v>26</v>
       </c>
       <c r="C118" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D118">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="E118">
         <v>8</v>
@@ -3005,7 +3059,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
-        <v>1.2855324074074075E-2</v>
+        <v>1.2877314814814814E-2</v>
       </c>
       <c r="B119" t="s">
         <v>26</v>
@@ -3022,33 +3076,33 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
-        <v>1.2877314814814814E-2</v>
+        <v>1.4348379629629628E-2</v>
       </c>
       <c r="B120" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C120" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D120">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="E120">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
-        <v>1.4348379629629628E-2</v>
+        <v>1.4355324074074074E-2</v>
       </c>
       <c r="B121" t="s">
         <v>27</v>
       </c>
       <c r="C121" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D121">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="E121">
         <v>9</v>
@@ -3056,16 +3110,16 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
-        <v>1.4355324074074074E-2</v>
+        <v>1.4386574074074072E-2</v>
       </c>
       <c r="B122" t="s">
         <v>27</v>
       </c>
       <c r="C122" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D122">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="E122">
         <v>9</v>
@@ -3073,16 +3127,16 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
-        <v>1.4386574074074072E-2</v>
+        <v>1.4407407407407409E-2</v>
       </c>
       <c r="B123" t="s">
         <v>27</v>
       </c>
       <c r="C123" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D123">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="E123">
         <v>9</v>
@@ -3090,16 +3144,16 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
-        <v>1.4407407407407409E-2</v>
+        <v>1.4424768518518519E-2</v>
       </c>
       <c r="B124" t="s">
         <v>27</v>
       </c>
       <c r="C124" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D124">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="E124">
         <v>9</v>
@@ -3107,16 +3161,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
-        <v>1.4424768518518519E-2</v>
+        <v>1.4438657407407409E-2</v>
       </c>
       <c r="B125" t="s">
         <v>27</v>
       </c>
       <c r="C125" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D125">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E125">
         <v>9</v>
@@ -3124,16 +3178,16 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
-        <v>1.4438657407407409E-2</v>
+        <v>1.4471064814814817E-2</v>
       </c>
       <c r="B126" t="s">
         <v>27</v>
       </c>
       <c r="C126" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D126">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E126">
         <v>9</v>
@@ -3141,16 +3195,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
-        <v>1.4471064814814817E-2</v>
+        <v>1.4519675925925927E-2</v>
       </c>
       <c r="B127" t="s">
         <v>27</v>
       </c>
       <c r="C127" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D127">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="E127">
         <v>9</v>
@@ -3158,16 +3212,16 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
-        <v>1.4519675925925927E-2</v>
+        <v>1.4538194444444444E-2</v>
       </c>
       <c r="B128" t="s">
         <v>27</v>
       </c>
       <c r="C128" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D128">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="E128">
         <v>9</v>
@@ -3175,16 +3229,16 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
-        <v>1.4538194444444444E-2</v>
+        <v>1.4550925925925925E-2</v>
       </c>
       <c r="B129" t="s">
         <v>27</v>
       </c>
       <c r="C129" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D129">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="E129">
         <v>9</v>
@@ -3192,16 +3246,16 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
-        <v>1.4550925925925925E-2</v>
+        <v>1.4556712962962964E-2</v>
       </c>
       <c r="B130" t="s">
         <v>27</v>
       </c>
       <c r="C130" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D130">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="E130">
         <v>9</v>
@@ -3209,16 +3263,16 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
-        <v>1.4556712962962964E-2</v>
+        <v>1.4574074074074074E-2</v>
       </c>
       <c r="B131" t="s">
         <v>27</v>
       </c>
       <c r="C131" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D131">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E131">
         <v>9</v>
@@ -3226,16 +3280,16 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
-        <v>1.4574074074074074E-2</v>
+        <v>1.4637731481481481E-2</v>
       </c>
       <c r="B132" t="s">
         <v>27</v>
       </c>
       <c r="C132" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D132">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="E132">
         <v>9</v>
@@ -3243,16 +3297,16 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
-        <v>1.4637731481481481E-2</v>
+        <v>1.466087962962963E-2</v>
       </c>
       <c r="B133" t="s">
         <v>27</v>
       </c>
       <c r="C133" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D133">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E133">
         <v>9</v>
@@ -3260,16 +3314,16 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
-        <v>1.466087962962963E-2</v>
+        <v>1.4726851851851852E-2</v>
       </c>
       <c r="B134" t="s">
         <v>27</v>
       </c>
       <c r="C134" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D134">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E134">
         <v>9</v>
@@ -3277,16 +3331,16 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
-        <v>1.4726851851851852E-2</v>
+        <v>1.4799768518518519E-2</v>
       </c>
       <c r="B135" t="s">
         <v>27</v>
       </c>
       <c r="C135" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D135">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E135">
         <v>9</v>
@@ -3294,16 +3348,16 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
-        <v>1.4799768518518519E-2</v>
+        <v>1.4814814814814814E-2</v>
       </c>
       <c r="B136" t="s">
         <v>27</v>
       </c>
       <c r="C136" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D136">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E136">
         <v>9</v>
@@ -3311,16 +3365,16 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
-        <v>1.4814814814814814E-2</v>
+        <v>1.4821759259259258E-2</v>
       </c>
       <c r="B137" t="s">
         <v>27</v>
       </c>
       <c r="C137" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D137">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E137">
         <v>9</v>
@@ -3328,16 +3382,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
-        <v>1.4821759259259258E-2</v>
+        <v>1.4854166666666667E-2</v>
       </c>
       <c r="B138" t="s">
         <v>27</v>
       </c>
       <c r="C138" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D138">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="E138">
         <v>9</v>
@@ -3345,16 +3399,16 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
-        <v>1.4854166666666667E-2</v>
+        <v>1.486689814814815E-2</v>
       </c>
       <c r="B139" t="s">
         <v>27</v>
       </c>
       <c r="C139" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D139">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="E139">
         <v>9</v>
@@ -3362,16 +3416,16 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
-        <v>1.486689814814815E-2</v>
+        <v>1.4887731481481481E-2</v>
       </c>
       <c r="B140" t="s">
         <v>27</v>
       </c>
       <c r="C140" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D140">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E140">
         <v>9</v>
@@ -3379,16 +3433,16 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
-        <v>1.4887731481481481E-2</v>
+        <v>1.489699074074074E-2</v>
       </c>
       <c r="B141" t="s">
         <v>27</v>
       </c>
       <c r="C141" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D141">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E141">
         <v>9</v>
@@ -3396,16 +3450,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
-        <v>1.489699074074074E-2</v>
+        <v>1.491087962962963E-2</v>
       </c>
       <c r="B142" t="s">
         <v>27</v>
       </c>
       <c r="C142" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D142">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="E142">
         <v>9</v>
@@ -3413,16 +3467,16 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
-        <v>1.491087962962963E-2</v>
+        <v>1.4920138888888887E-2</v>
       </c>
       <c r="B143" t="s">
         <v>27</v>
       </c>
       <c r="C143" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D143">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="E143">
         <v>9</v>
@@ -3430,7 +3484,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
-        <v>1.4920138888888887E-2</v>
+        <v>1.4927083333333334E-2</v>
       </c>
       <c r="B144" t="s">
         <v>27</v>
@@ -3447,7 +3501,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
-        <v>1.4927083333333334E-2</v>
+        <v>1.4936342592592591E-2</v>
       </c>
       <c r="B145" t="s">
         <v>27</v>
@@ -3464,7 +3518,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
-        <v>1.4936342592592591E-2</v>
+        <v>1.5042824074074075E-2</v>
       </c>
       <c r="B146" t="s">
         <v>27</v>
@@ -3481,33 +3535,33 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
-        <v>1.5042824074074075E-2</v>
+        <v>1.5221064814814814E-2</v>
       </c>
       <c r="B147" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C147" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D147">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E147">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
-        <v>1.5221064814814814E-2</v>
+        <v>1.5318287037037038E-2</v>
       </c>
       <c r="B148" t="s">
         <v>28</v>
       </c>
       <c r="C148" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D148">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="E148">
         <v>10</v>
@@ -3515,16 +3569,16 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
-        <v>1.5318287037037038E-2</v>
+        <v>1.5329861111111112E-2</v>
       </c>
       <c r="B149" t="s">
         <v>28</v>
       </c>
       <c r="C149" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D149">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="E149">
         <v>10</v>
@@ -3532,16 +3586,16 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
-        <v>1.5329861111111112E-2</v>
+        <v>1.541898148148148E-2</v>
       </c>
       <c r="B150" t="s">
         <v>28</v>
       </c>
       <c r="C150" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D150">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E150">
         <v>10</v>
@@ -3549,16 +3603,16 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
-        <v>1.541898148148148E-2</v>
+        <v>1.5478009259259261E-2</v>
       </c>
       <c r="B151" t="s">
         <v>28</v>
       </c>
       <c r="C151" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D151">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E151">
         <v>10</v>
@@ -3566,16 +3620,16 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
-        <v>1.5478009259259261E-2</v>
+        <v>1.5498842592592594E-2</v>
       </c>
       <c r="B152" t="s">
         <v>28</v>
       </c>
       <c r="C152" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D152">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E152">
         <v>10</v>
@@ -3583,16 +3637,16 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
-        <v>1.5498842592592594E-2</v>
+        <v>1.551851851851852E-2</v>
       </c>
       <c r="B153" t="s">
         <v>28</v>
       </c>
       <c r="C153" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D153">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E153">
         <v>10</v>
@@ -3600,16 +3654,16 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
-        <v>1.551851851851852E-2</v>
+        <v>1.5525462962962963E-2</v>
       </c>
       <c r="B154" t="s">
         <v>28</v>
       </c>
       <c r="C154" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D154">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E154">
         <v>10</v>
@@ -3617,16 +3671,16 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
-        <v>1.5525462962962963E-2</v>
+        <v>1.5537037037037038E-2</v>
       </c>
       <c r="B155" t="s">
         <v>28</v>
       </c>
       <c r="C155" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D155">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E155">
         <v>10</v>
@@ -3634,16 +3688,16 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
-        <v>1.5537037037037038E-2</v>
+        <v>1.5547453703703702E-2</v>
       </c>
       <c r="B156" t="s">
         <v>28</v>
       </c>
       <c r="C156" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D156">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E156">
         <v>10</v>
@@ -3651,16 +3705,16 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
-        <v>1.5547453703703702E-2</v>
+        <v>1.5552083333333333E-2</v>
       </c>
       <c r="B157" t="s">
         <v>28</v>
       </c>
       <c r="C157" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D157">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E157">
         <v>10</v>
@@ -3668,16 +3722,16 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
-        <v>1.5552083333333333E-2</v>
+        <v>1.5568287037037038E-2</v>
       </c>
       <c r="B158" t="s">
         <v>28</v>
       </c>
       <c r="C158" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D158">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="E158">
         <v>10</v>
@@ -3685,16 +3739,16 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
-        <v>1.5568287037037038E-2</v>
+        <v>1.5594907407407406E-2</v>
       </c>
       <c r="B159" t="s">
         <v>28</v>
       </c>
       <c r="C159" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D159">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="E159">
         <v>10</v>
@@ -3702,16 +3756,16 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
-        <v>1.5594907407407406E-2</v>
+        <v>1.5614583333333333E-2</v>
       </c>
       <c r="B160" t="s">
         <v>28</v>
       </c>
       <c r="C160" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D160">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E160">
         <v>10</v>
@@ -3719,16 +3773,16 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
-        <v>1.5614583333333333E-2</v>
+        <v>1.5618055555555553E-2</v>
       </c>
       <c r="B161" t="s">
         <v>28</v>
       </c>
       <c r="C161" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D161">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E161">
         <v>10</v>
@@ -3736,16 +3790,16 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
-        <v>1.5618055555555553E-2</v>
+        <v>1.5675925925925926E-2</v>
       </c>
       <c r="B162" t="s">
         <v>28</v>
       </c>
       <c r="C162" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D162">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="E162">
         <v>10</v>
@@ -3753,16 +3807,16 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
-        <v>1.5675925925925926E-2</v>
+        <v>1.5693287037037037E-2</v>
       </c>
       <c r="B163" t="s">
         <v>28</v>
       </c>
       <c r="C163" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D163">
-        <v>91</v>
+        <v>6</v>
       </c>
       <c r="E163">
         <v>10</v>
@@ -3770,16 +3824,16 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
-        <v>1.5693287037037037E-2</v>
+        <v>1.5806712962962963E-2</v>
       </c>
       <c r="B164" t="s">
         <v>28</v>
       </c>
       <c r="C164" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D164">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E164">
         <v>10</v>
@@ -3787,7 +3841,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
-        <v>1.5806712962962963E-2</v>
+        <v>1.5915509259259258E-2</v>
       </c>
       <c r="B165" t="s">
         <v>28</v>
@@ -3807,7 +3861,7 @@
         <v>1.5915509259259258E-2</v>
       </c>
       <c r="B166" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C166" t="s">
         <v>14</v>
@@ -3816,21 +3870,21 @@
         <v>18</v>
       </c>
       <c r="E166">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
-        <v>1.5915509259259258E-2</v>
+        <v>1.5922453703703706E-2</v>
       </c>
       <c r="B167" t="s">
         <v>29</v>
       </c>
       <c r="C167" t="s">
+        <v>19</v>
+      </c>
+      <c r="D167">
         <v>14</v>
-      </c>
-      <c r="D167">
-        <v>18</v>
       </c>
       <c r="E167">
         <v>11</v>
@@ -3838,16 +3892,16 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
-        <v>1.5922453703703706E-2</v>
+        <v>1.5935185185185184E-2</v>
       </c>
       <c r="B168" t="s">
         <v>29</v>
       </c>
       <c r="C168" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D168">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E168">
         <v>11</v>
@@ -3855,7 +3909,7 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
-        <v>1.5935185185185184E-2</v>
+        <v>1.6609953703703703E-2</v>
       </c>
       <c r="B169" t="s">
         <v>29</v>
@@ -3872,10 +3926,10 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
-        <v>1.6609953703703703E-2</v>
+        <v>1.7719907407407406E-2</v>
       </c>
       <c r="B170" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C170" t="s">
         <v>7</v>
@@ -3884,21 +3938,21 @@
         <v>1</v>
       </c>
       <c r="E170">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
-        <v>1.7719907407407406E-2</v>
+        <v>1.776273148148148E-2</v>
       </c>
       <c r="B171" t="s">
         <v>30</v>
       </c>
       <c r="C171" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D171">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E171">
         <v>12</v>
@@ -3906,16 +3960,16 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
-        <v>1.776273148148148E-2</v>
+        <v>1.7872685185185186E-2</v>
       </c>
       <c r="B172" t="s">
         <v>30</v>
       </c>
       <c r="C172" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D172">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E172">
         <v>12</v>
@@ -3923,16 +3977,16 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
-        <v>1.7872685185185186E-2</v>
+        <v>1.7880787037037039E-2</v>
       </c>
       <c r="B173" t="s">
         <v>30</v>
       </c>
       <c r="C173" t="s">
+        <v>20</v>
+      </c>
+      <c r="D173">
         <v>6</v>
-      </c>
-      <c r="D173">
-        <v>30</v>
       </c>
       <c r="E173">
         <v>12</v>
@@ -3940,16 +3994,16 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
-        <v>1.7880787037037039E-2</v>
+        <v>1.8115740740740741E-2</v>
       </c>
       <c r="B174" t="s">
         <v>30</v>
       </c>
       <c r="C174" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D174">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E174">
         <v>12</v>
@@ -3957,16 +4011,16 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
-        <v>1.8115740740740741E-2</v>
+        <v>1.8129629629629631E-2</v>
       </c>
       <c r="B175" t="s">
         <v>30</v>
       </c>
       <c r="C175" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D175">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E175">
         <v>12</v>
@@ -3974,16 +4028,16 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
-        <v>1.8129629629629631E-2</v>
+        <v>1.8135416666666664E-2</v>
       </c>
       <c r="B176" t="s">
         <v>30</v>
       </c>
       <c r="C176" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D176">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="E176">
         <v>12</v>
@@ -3991,16 +4045,16 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
-        <v>1.8135416666666664E-2</v>
+        <v>1.8210648148148146E-2</v>
       </c>
       <c r="B177" t="s">
         <v>30</v>
       </c>
       <c r="C177" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D177">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E177">
         <v>12</v>
@@ -4008,16 +4062,16 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
-        <v>1.8210648148148146E-2</v>
+        <v>1.8216435185185186E-2</v>
       </c>
       <c r="B178" t="s">
         <v>30</v>
       </c>
       <c r="C178" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D178">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E178">
         <v>12</v>
@@ -4025,16 +4079,16 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
-        <v>1.8216435185185186E-2</v>
+        <v>1.8225694444444444E-2</v>
       </c>
       <c r="B179" t="s">
         <v>30</v>
       </c>
       <c r="C179" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D179">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E179">
         <v>12</v>
@@ -4042,16 +4096,16 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
-        <v>1.8225694444444444E-2</v>
+        <v>1.8337962962962962E-2</v>
       </c>
       <c r="B180" t="s">
         <v>30</v>
       </c>
       <c r="C180" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D180">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E180">
         <v>12</v>
@@ -4059,16 +4113,16 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
-        <v>1.8337962962962962E-2</v>
+        <v>1.8343749999999999E-2</v>
       </c>
       <c r="B181" t="s">
         <v>30</v>
       </c>
       <c r="C181" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D181">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E181">
         <v>12</v>
@@ -4076,16 +4130,16 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
-        <v>1.8343749999999999E-2</v>
+        <v>1.8357638888888889E-2</v>
       </c>
       <c r="B182" t="s">
         <v>30</v>
       </c>
       <c r="C182" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D182">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E182">
         <v>12</v>
@@ -4093,16 +4147,16 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
-        <v>1.8357638888888889E-2</v>
+        <v>1.8380787037037039E-2</v>
       </c>
       <c r="B183" t="s">
         <v>30</v>
       </c>
       <c r="C183" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D183">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E183">
         <v>12</v>
@@ -4110,16 +4164,16 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
-        <v>1.8380787037037039E-2</v>
+        <v>1.8413194444444444E-2</v>
       </c>
       <c r="B184" t="s">
         <v>30</v>
       </c>
       <c r="C184" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D184">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E184">
         <v>12</v>
@@ -4127,7 +4181,7 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
-        <v>1.8413194444444444E-2</v>
+        <v>1.8414351851851852E-2</v>
       </c>
       <c r="B185" t="s">
         <v>30</v>
@@ -4144,33 +4198,33 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
-        <v>1.8414351851851852E-2</v>
+        <v>1.886689814814815E-2</v>
       </c>
       <c r="B186" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C186" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D186">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="E186">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" s="1">
-        <v>1.886689814814815E-2</v>
+        <v>1.8952546296296297E-2</v>
       </c>
       <c r="B187" t="s">
         <v>31</v>
       </c>
       <c r="C187" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D187">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E187">
         <v>13</v>
@@ -4178,16 +4232,16 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" s="1">
-        <v>1.8952546296296297E-2</v>
+        <v>1.897800925925926E-2</v>
       </c>
       <c r="B188" t="s">
         <v>31</v>
       </c>
       <c r="C188" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D188">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E188">
         <v>13</v>
@@ -4195,16 +4249,16 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" s="1">
-        <v>1.897800925925926E-2</v>
+        <v>1.8983796296296294E-2</v>
       </c>
       <c r="B189" t="s">
         <v>31</v>
       </c>
       <c r="C189" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D189">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E189">
         <v>13</v>
@@ -4212,16 +4266,16 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" s="1">
-        <v>1.8983796296296294E-2</v>
+        <v>1.8998842592592591E-2</v>
       </c>
       <c r="B190" t="s">
         <v>31</v>
       </c>
       <c r="C190" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D190">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E190">
         <v>13</v>
@@ -4229,16 +4283,16 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" s="1">
-        <v>1.8998842592592591E-2</v>
+        <v>1.9006944444444444E-2</v>
       </c>
       <c r="B191" t="s">
         <v>31</v>
       </c>
       <c r="C191" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D191">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E191">
         <v>13</v>
@@ -4246,16 +4300,16 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="1">
-        <v>1.9006944444444444E-2</v>
+        <v>1.9027777777777779E-2</v>
       </c>
       <c r="B192" t="s">
         <v>31</v>
       </c>
       <c r="C192" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D192">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E192">
         <v>13</v>
@@ -4263,16 +4317,16 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="1">
-        <v>1.9027777777777779E-2</v>
+        <v>1.9163194444444445E-2</v>
       </c>
       <c r="B193" t="s">
         <v>31</v>
       </c>
       <c r="C193" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D193">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E193">
         <v>13</v>
@@ -4280,16 +4334,16 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="1">
-        <v>1.9163194444444445E-2</v>
+        <v>1.9185185185185184E-2</v>
       </c>
       <c r="B194" t="s">
         <v>31</v>
       </c>
       <c r="C194" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D194">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E194">
         <v>13</v>
@@ -4297,16 +4351,16 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="1">
-        <v>1.9185185185185184E-2</v>
+        <v>1.9234953703703702E-2</v>
       </c>
       <c r="B195" t="s">
         <v>31</v>
       </c>
       <c r="C195" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D195">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E195">
         <v>13</v>
@@ -4314,16 +4368,16 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="1">
-        <v>1.9234953703703702E-2</v>
+        <v>1.9263888888888889E-2</v>
       </c>
       <c r="B196" t="s">
         <v>31</v>
       </c>
       <c r="C196" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D196">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E196">
         <v>13</v>
@@ -4331,7 +4385,7 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="1">
-        <v>1.9263888888888889E-2</v>
+        <v>1.9561342592592592E-2</v>
       </c>
       <c r="B197" t="s">
         <v>31</v>
@@ -4347,24 +4401,619 @@
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A198" s="1">
-        <v>1.9561342592592592E-2</v>
-      </c>
-      <c r="B198" t="s">
+      <c r="A198" s="2">
+        <v>1.0141203703703704E-2</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C198" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D198" s="5">
+        <v>1</v>
+      </c>
+      <c r="E198">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A199" s="2">
+        <v>1.0190972222222225E-2</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C199" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D199" s="4">
         <v>31</v>
       </c>
-      <c r="C198" t="s">
-        <v>7</v>
-      </c>
-      <c r="D198">
-        <v>1</v>
-      </c>
-      <c r="E198">
+      <c r="E199">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A200" s="2">
+        <v>1.0230324074074074E-2</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C200" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D200" s="5">
+        <v>30</v>
+      </c>
+      <c r="E200">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A201" s="2">
+        <v>1.0266203703703703E-2</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C201" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D201" s="5">
+        <v>31</v>
+      </c>
+      <c r="E201">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A202" s="2">
+        <v>1.0280092592592592E-2</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C202" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D202" s="5">
+        <v>1</v>
+      </c>
+      <c r="E202">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A203" s="2">
+        <v>1.0581018518518517E-2</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C203" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D203" s="4">
+        <v>31</v>
+      </c>
+      <c r="E203">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A204" s="2">
+        <v>1.0607638888888889E-2</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C204" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D204" s="5">
+        <v>1</v>
+      </c>
+      <c r="E204">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A205" s="2">
+        <v>1.0831018518518518E-2</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C205" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D205" s="4">
+        <v>14</v>
+      </c>
+      <c r="E205">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A206" s="2">
+        <v>1.0835648148148148E-2</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C206" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D206" s="5">
+        <v>1</v>
+      </c>
+      <c r="E206">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A207" s="2">
+        <v>3.2152777777777774E-3</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C207" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D207" s="5">
+        <v>1</v>
+      </c>
+      <c r="E207">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A208" s="2">
+        <v>3.3680555555555556E-3</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C208" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D208" s="4">
+        <v>2</v>
+      </c>
+      <c r="E208">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A209" s="2">
+        <v>3.3854166666666676E-3</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C209" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D209" s="5">
+        <v>1</v>
+      </c>
+      <c r="E209">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A210" s="2">
+        <v>3.4375000000000005E-3</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C210" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D210" s="4">
         <v>13</v>
       </c>
+      <c r="E210">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A211" s="2">
+        <v>3.4432870370370372E-3</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C211" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D211" s="5">
+        <v>1</v>
+      </c>
+      <c r="E211">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A212" s="2">
+        <v>3.4756944444444444E-3</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C212" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D212" s="4">
+        <v>30</v>
+      </c>
+      <c r="E212">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A213" s="2">
+        <v>3.4895833333333333E-3</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C213" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D213" s="5">
+        <v>1</v>
+      </c>
+      <c r="E213">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A214" s="2">
+        <v>3.6064814814814813E-3</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C214" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D214" s="4">
+        <v>91</v>
+      </c>
+      <c r="E214">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A215" s="2">
+        <v>3.6157407407407414E-3</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C215" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D215" s="5">
+        <v>1</v>
+      </c>
+      <c r="E215">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A216" s="2">
+        <v>3.7499999999999999E-3</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C216" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D216" s="4">
+        <v>2</v>
+      </c>
+      <c r="E216">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A217" s="2">
+        <v>3.7731481481481479E-3</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C217" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D217" s="5">
+        <v>1</v>
+      </c>
+      <c r="E217">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A218" s="2">
+        <v>3.8657407407407416E-3</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C218" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D218" s="4">
+        <v>7</v>
+      </c>
+      <c r="E218">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A219" s="2">
+        <v>3.8854166666666664E-3</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C219" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D219" s="5">
+        <v>1</v>
+      </c>
+      <c r="E219">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A220" s="2">
+        <v>3.9097222222222224E-3</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C220" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D220" s="5">
+        <v>1</v>
+      </c>
+      <c r="E220">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A221" s="2">
+        <v>1.9967592592592592E-2</v>
+      </c>
+      <c r="B221" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C221" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D221" s="5">
+        <v>1</v>
+      </c>
+      <c r="E221">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A222" s="2">
+        <v>1.9983796296296298E-2</v>
+      </c>
+      <c r="B222" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C222" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D222" s="4">
+        <v>8</v>
+      </c>
+      <c r="E222">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A223" s="2">
+        <v>2.0047453703703706E-2</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C223" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D223" s="5">
+        <v>1</v>
+      </c>
+      <c r="E223">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A224" s="2">
+        <v>2.009027777777778E-2</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C224" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D224" s="4">
+        <v>18</v>
+      </c>
+      <c r="E224">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A225" s="2">
+        <v>2.0103009259259261E-2</v>
+      </c>
+      <c r="B225" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C225" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D225" s="5">
+        <v>1</v>
+      </c>
+      <c r="E225">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A226" s="2">
+        <v>2.0111111111111111E-2</v>
+      </c>
+      <c r="B226" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C226" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D226" s="4">
+        <v>8</v>
+      </c>
+      <c r="E226">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A227" s="2">
+        <v>2.0200231481481486E-2</v>
+      </c>
+      <c r="B227" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C227" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D227" s="4">
+        <v>2</v>
+      </c>
+      <c r="E227">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A228" s="2">
+        <v>2.0221064814814813E-2</v>
+      </c>
+      <c r="B228" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C228" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D228" s="4">
+        <v>13</v>
+      </c>
+      <c r="E228">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A229" s="2">
+        <v>2.0234953703703703E-2</v>
+      </c>
+      <c r="B229" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C229" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D229" s="4">
+        <v>31</v>
+      </c>
+      <c r="E229">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A230" s="2">
+        <v>2.0288194444444446E-2</v>
+      </c>
+      <c r="B230" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C230" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D230" s="5">
+        <v>30</v>
+      </c>
+      <c r="E230">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A231" s="2">
+        <v>2.0311342592592593E-2</v>
+      </c>
+      <c r="B231" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C231" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D231" s="5">
+        <v>1</v>
+      </c>
+      <c r="E231">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A232" s="2">
+        <v>2.0559027777777777E-2</v>
+      </c>
+      <c r="B232" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C232" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D232" s="4">
+        <v>31</v>
+      </c>
+      <c r="E232">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A233" s="2">
+        <v>2.0662037037037038E-2</v>
+      </c>
+      <c r="B233" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C233" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D233" s="4">
+        <v>31</v>
+      </c>
+      <c r="E233">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:XEX198" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:XEX197" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>